<commit_message>
todo listo ahora si
</commit_message>
<xml_diff>
--- a/Matriz Compiladores.xlsx
+++ b/Matriz Compiladores.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fermin\Dropbox\Facultad grego\Cuarto\Segundo Cuatrimestre\Diseño de Compiladores\TP Compiladores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fermin\Documents\GitHub\compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="21570" windowHeight="8085"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="21570" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="28">
   <si>
     <t>_</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>"</t>
+  </si>
+  <si>
+    <t>FinSimbolo</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -207,10 +210,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -219,16 +228,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -513,11 +513,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:E2"/>
+      <selection pane="bottomRight" activeCell="R8" sqref="B8:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,81 +535,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="11">
         <v>0</v>
       </c>
       <c r="B3" s="1">
@@ -665,7 +665,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
@@ -719,7 +719,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="11">
         <v>1</v>
       </c>
       <c r="B5" s="1">
@@ -775,7 +775,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
@@ -829,7 +829,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="11">
         <v>2</v>
       </c>
       <c r="B7" s="1">
@@ -885,61 +885,61 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="11">
         <v>3</v>
       </c>
       <c r="B9" s="1">
@@ -995,7 +995,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1049,7 +1049,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="11">
         <v>4</v>
       </c>
       <c r="B11" s="1">
@@ -1105,7 +1105,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1159,7 +1159,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="11">
         <v>5</v>
       </c>
       <c r="B13" s="1">
@@ -1215,7 +1215,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -1269,7 +1269,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="11">
         <v>6</v>
       </c>
       <c r="B15" s="1">
@@ -1325,7 +1325,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="11">
         <v>7</v>
       </c>
       <c r="B17" s="1">
@@ -1435,7 +1435,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
@@ -1489,7 +1489,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="11">
         <v>8</v>
       </c>
       <c r="B19" s="1">
@@ -1545,7 +1545,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
@@ -1599,7 +1599,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="11">
         <v>9</v>
       </c>
       <c r="B21" s="1">
@@ -1655,7 +1655,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
@@ -1709,7 +1709,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="A23" s="11">
         <v>10</v>
       </c>
       <c r="B23" s="1">
@@ -1765,7 +1765,7 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="3" t="s">
         <v>17</v>
       </c>
@@ -1819,7 +1819,7 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+      <c r="A25" s="11">
         <v>11</v>
       </c>
       <c r="B25" s="1">
@@ -1875,7 +1875,7 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
@@ -1929,7 +1929,7 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+      <c r="A27" s="11">
         <v>12</v>
       </c>
       <c r="B27" s="1">
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
@@ -2039,7 +2039,7 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+      <c r="A29" s="11">
         <v>13</v>
       </c>
       <c r="B29" s="1">
@@ -2095,7 +2095,7 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="3" t="s">
         <v>17</v>
       </c>
@@ -2149,7 +2149,7 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="A31" s="11">
         <v>14</v>
       </c>
       <c r="B31" s="1">
@@ -2205,7 +2205,7 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="3" t="s">
         <v>20</v>
       </c>
@@ -2260,23 +2260,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
@@ -2293,6 +2276,23 @@
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>